<commit_message>
Major update of the structure. Attendences.csv reviewed.
</commit_message>
<xml_diff>
--- a/Files/Attendances.xlsx
+++ b/Files/Attendances.xlsx
@@ -5,19 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Attendances" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Aug-Dec" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Final" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Pos</t>
   </si>
@@ -146,6 +147,84 @@
   </si>
   <si>
     <t>−36.5%</t>
+  </si>
+  <si>
+    <t>+11.1%</t>
+  </si>
+  <si>
+    <t>+6.9%</t>
+  </si>
+  <si>
+    <t>+14.8%</t>
+  </si>
+  <si>
+    <t>+50.9%</t>
+  </si>
+  <si>
+    <t>+2.9%</t>
+  </si>
+  <si>
+    <t>+27.2%</t>
+  </si>
+  <si>
+    <t>+5.9%</t>
+  </si>
+  <si>
+    <t>−9.2%</t>
+  </si>
+  <si>
+    <t>+19.7%</t>
+  </si>
+  <si>
+    <t>−13.3%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">+33.3%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[1]</t>
+    </r>
+  </si>
+  <si>
+    <t>+21.9%</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">+183.5%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[1]</t>
+    </r>
+  </si>
+  <si>
+    <t>+9.8%</t>
+  </si>
+  <si>
+    <t>−30.5%</t>
+  </si>
+  <si>
+    <t>−22.6%</t>
+  </si>
+  <si>
+    <t>−2.0%</t>
+  </si>
+  <si>
+    <t>−40.7%</t>
   </si>
 </sst>
 </file>
@@ -157,7 +236,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -190,6 +269,20 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -235,7 +328,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -253,6 +346,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,7 +385,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:F19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -302,7 +411,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:F19 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -327,8 +436,8 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:F19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -782,4 +891,474 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>951184</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>64591</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>46256</v>
+      </c>
+      <c r="F2" s="7" t="n">
+        <v>55952</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>727121</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>49399</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <v>32457</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>42772</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>631202</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>50019</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>22208</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>37130</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>318856</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>26985</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <v>12953</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>18756</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>195366</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>24836</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>5545</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>11492</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>132909</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>10454</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>4150</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>7818</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>103461</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>16157</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>3955</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>6086</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>68799</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>12236</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>1309</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>4047</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>67215</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>8767</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>1508</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>3954</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="6" t="n">
+        <v>65320</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>10109</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>2081</v>
+      </c>
+      <c r="F11" s="7" t="n">
+        <v>3842</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>61551</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>8000</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>1730</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <v>3496</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="n">
+        <v>58051</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>9076</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>1059</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <v>3415</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="n">
+        <v>50517</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>5449</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <v>1099</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <v>2972</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6" t="n">
+        <v>46500</v>
+      </c>
+      <c r="D15" s="6" t="n">
+        <v>5017</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>1126</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>2735</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="6" t="n">
+        <v>39239</v>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>4987</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>1045</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <v>2308</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="6" t="n">
+        <v>38668</v>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>7429</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>877</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <v>2275</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="6" t="n">
+        <v>37383</v>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>5603</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>640</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <v>2199</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>29030</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>5351</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>658</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>1708</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G12" r:id="rId1" location="endnote_Promotion" display="[1]"/>
+    <hyperlink ref="G14" r:id="rId2" location="endnote_Promotion" display="[1]"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>